<commit_message>
I added bump case as well as some other material constants and final report
</commit_message>
<xml_diff>
--- a/Arm_Materials.xlsx
+++ b/Arm_Materials.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william_hess/Desktop/FSAE/taiyangie-LinkageForceAnalyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD3C14C-D236-514E-80CC-D1B3F6413774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923B4744-F1BF-B940-BDA5-54AF8D9BBDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="500" windowWidth="18960" windowHeight="16440" xr2:uid="{032B2732-D4ED-D941-8495-B4A5262353BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Points</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>Density (lb/in^3)</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CA1E4D-4640-8348-A2A4-19EFD0683612}">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -1383,6 +1386,83 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="C11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="D11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="F11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="G11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="H11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="I11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="J11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="K11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="L11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="M11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="N11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="O11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="P11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="Q11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="R11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="S11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="T11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="U11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="V11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="W11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="X11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="Y11">
+        <v>0.28399999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>